<commit_message>
fixed no fault data
</commit_message>
<xml_diff>
--- a/nofault/nofault_data/data_nofault_M.xlsx
+++ b/nofault/nofault_data/data_nofault_M.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fguo/Documents/GitHub/SimpleStorageSystem/nofault/nofault_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868A0C13-4508-524B-8437-71ECFACB2D3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4B51BF-6A1B-3947-B050-B46C8FFE59A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19320" yWindow="460" windowWidth="14280" windowHeight="19080" xr2:uid="{47B0A791-D727-6445-83EF-50FD20C84FF4}"/>
   </bookViews>
@@ -434,12 +434,12 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -470,7 +470,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1">
         <v>10</v>
@@ -479,13 +479,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>284</v>
+        <v>942</v>
       </c>
       <c r="F2" s="1">
-        <v>59385</v>
+        <v>19703384</v>
       </c>
       <c r="G2" s="1">
-        <v>28927783</v>
+        <v>92519041</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -493,7 +493,7 @@
         <v>100</v>
       </c>
       <c r="B3" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C3" s="1">
         <v>10</v>
@@ -502,13 +502,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1">
-        <v>486</v>
+        <v>1551</v>
       </c>
       <c r="F3" s="1">
-        <v>94214</v>
+        <v>35722808</v>
       </c>
       <c r="G3" s="1">
-        <v>38074621</v>
+        <v>94016619</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -516,7 +516,7 @@
         <v>150</v>
       </c>
       <c r="B4" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C4" s="1">
         <v>10</v>
@@ -525,13 +525,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>713</v>
+        <v>2154</v>
       </c>
       <c r="F4" s="1">
-        <v>155848</v>
+        <v>56203784</v>
       </c>
       <c r="G4" s="1">
-        <v>37112278</v>
+        <v>98854219</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -539,7 +539,7 @@
         <v>200</v>
       </c>
       <c r="B5" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C5" s="1">
         <v>10</v>
@@ -548,13 +548,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>898</v>
+        <v>2633</v>
       </c>
       <c r="F5" s="1">
-        <v>175483</v>
+        <v>73843544</v>
       </c>
       <c r="G5" s="1">
-        <v>33472465</v>
+        <v>103817289</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -562,7 +562,7 @@
         <v>250</v>
       </c>
       <c r="B6" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C6" s="1">
         <v>10</v>
@@ -571,13 +571,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1">
-        <v>1100</v>
+        <v>3243</v>
       </c>
       <c r="F6" s="1">
-        <v>194889</v>
+        <v>96230776</v>
       </c>
       <c r="G6" s="1">
-        <v>36539908</v>
+        <v>111838396</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -585,7 +585,7 @@
         <v>300</v>
       </c>
       <c r="B7" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C7" s="1">
         <v>10</v>
@@ -594,13 +594,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1">
-        <v>1286</v>
+        <v>3706</v>
       </c>
       <c r="F7" s="1">
-        <v>214307</v>
+        <v>113592304</v>
       </c>
       <c r="G7" s="1">
-        <v>40659119</v>
+        <v>133722718</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -608,7 +608,7 @@
         <v>350</v>
       </c>
       <c r="B8" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C8" s="1">
         <v>10</v>
@@ -617,13 +617,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1">
-        <v>1479</v>
+        <v>4227</v>
       </c>
       <c r="F8" s="1">
-        <v>231165</v>
+        <v>128964976</v>
       </c>
       <c r="G8" s="1">
-        <v>54991502</v>
+        <v>188760946</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -631,7 +631,7 @@
         <v>400</v>
       </c>
       <c r="B9" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C9" s="1">
         <v>10</v>
@@ -640,13 +640,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>1708</v>
+        <v>4788</v>
       </c>
       <c r="F9" s="1">
-        <v>317667</v>
+        <v>149534432</v>
       </c>
       <c r="G9" s="1">
-        <v>53618889</v>
+        <v>170682100</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -654,7 +654,7 @@
         <v>450</v>
       </c>
       <c r="B10" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C10" s="1">
         <v>10</v>
@@ -663,13 +663,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1">
-        <v>1884</v>
+        <v>5174</v>
       </c>
       <c r="F10" s="1">
-        <v>311188</v>
+        <v>164975200</v>
       </c>
       <c r="G10" s="1">
-        <v>59368081</v>
+        <v>184293197</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -677,7 +677,7 @@
         <v>500</v>
       </c>
       <c r="B11" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C11" s="1">
         <v>10</v>
@@ -686,13 +686,13 @@
         <v>1</v>
       </c>
       <c r="E11" s="1">
-        <v>2107</v>
+        <v>5894</v>
       </c>
       <c r="F11" s="1">
-        <v>382008</v>
+        <v>186626800</v>
       </c>
       <c r="G11" s="1">
-        <v>66739717</v>
+        <v>277777750</v>
       </c>
     </row>
     <row r="12" spans="1:7">

</xml_diff>